<commit_message>
many changes, latest being adding course attrs to custom model and multifilter
</commit_message>
<xml_diff>
--- a/DataCaddie/data/field_strength/StrengthOfField.xlsx
+++ b/DataCaddie/data/field_strength/StrengthOfField.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sethjernigan/Desktop/DataCaddie/DataCaddieShiny/DataCaddie/data/field_strength/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469F010A-76C0-EF41-B94F-F32FEC1E942E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569BAA53-DCD5-E042-A90E-CF0AC5593C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28380" yWindow="3040" windowWidth="23260" windowHeight="13900" xr2:uid="{393FFEE0-6F55-406A-94E7-E3110FEB23F9}"/>
+    <workbookView xWindow="17380" yWindow="920" windowWidth="17040" windowHeight="20200" xr2:uid="{393FFEE0-6F55-406A-94E7-E3110FEB23F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>Genesis Scottish Open</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Rocket Classic</t>
+  </si>
+  <si>
+    <t>Bank of Utah Championship</t>
   </si>
 </sst>
 </file>
@@ -551,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB66AC3-CA22-43F7-ACA6-12512B713D05}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1487,6 +1490,72 @@
         <v>-0.25</v>
       </c>
     </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85">
+        <v>2025</v>
+      </c>
+      <c r="C85">
+        <v>-0.35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>48</v>
+      </c>
+      <c r="B86">
+        <v>2025</v>
+      </c>
+      <c r="C86">
+        <v>-0.43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87">
+        <v>2025</v>
+      </c>
+      <c r="C87">
+        <v>-0.44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88">
+        <v>2025</v>
+      </c>
+      <c r="C88">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89">
+        <v>2026</v>
+      </c>
+      <c r="C89">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90">
+        <v>2026</v>
+      </c>
+      <c r="C90">
+        <v>0.11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>